<commit_message>
speculative coverage cleaned, all the control treatments combined (by using `summarize` instead of `mutate`)
</commit_message>
<xml_diff>
--- a/2-Data/Raw/Rawdata_FSBrassica_RA.team.xlsx
+++ b/2-Data/Raw/Rawdata_FSBrassica_RA.team.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20386"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryanlab\Box\SCS lab share\Biomass Weighing 2021 &amp; 2022, RA access\FSB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hn337/Library/CloudStorage/Box-Box/SCS lab share/Biomass Weighing 2021 &amp; 2022, RA access/FSB (brassicas)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D541365F-3B1A-439F-B63F-1D1FFC2F5B64}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48A7399-0E9D-3B45-B3DE-9C8B6C7B97AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18312" windowHeight="7560" xr2:uid="{F53A1BFA-809E-4EDF-B6BA-4084135DB466}"/>
+    <workbookView xWindow="20640" yWindow="1140" windowWidth="18320" windowHeight="7560" activeTab="1" xr2:uid="{F53A1BFA-809E-4EDF-B6BA-4084135DB466}"/>
   </bookViews>
   <sheets>
     <sheet name="Biomass" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="134">
   <si>
     <t>Block 1</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>FSB-4_A_Radish</t>
+  </si>
+  <si>
+    <t>Speculative % Cover</t>
   </si>
 </sst>
 </file>
@@ -830,17 +833,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21FA43B-595D-4FBD-B18C-E97882B90318}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+    <sheetView zoomScale="95" workbookViewId="0">
       <selection activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -857,7 +860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -871,7 +874,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -885,7 +888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -899,7 +902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -914,7 +917,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -928,7 +931,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -942,7 +945,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -953,7 +956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -964,7 +967,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -975,7 +978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -986,7 +989,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -1019,7 +1022,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -1030,7 +1033,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1041,7 +1044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -1052,7 +1055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -1063,7 +1066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -1074,7 +1077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -1085,7 +1088,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
@@ -1096,7 +1099,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
@@ -1107,7 +1110,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>29</v>
       </c>
@@ -1118,7 +1121,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>30</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
@@ -1140,7 +1143,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>32</v>
       </c>
@@ -1151,7 +1154,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>33</v>
       </c>
@@ -1162,7 +1165,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>34</v>
       </c>
@@ -1173,7 +1176,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>99</v>
       </c>
@@ -1184,7 +1187,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>100</v>
       </c>
@@ -1195,7 +1198,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>35</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
@@ -1217,7 +1220,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -1228,7 +1231,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>38</v>
       </c>
@@ -1239,7 +1242,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>39</v>
       </c>
@@ -1250,7 +1253,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>40</v>
       </c>
@@ -1261,7 +1264,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>41</v>
       </c>
@@ -1272,7 +1275,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>42</v>
       </c>
@@ -1283,7 +1286,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>43</v>
       </c>
@@ -1294,7 +1297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>44</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>45</v>
       </c>
@@ -1316,7 +1319,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>46</v>
       </c>
@@ -1327,7 +1330,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>49</v>
       </c>
@@ -1349,7 +1352,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>50</v>
       </c>
@@ -1360,7 +1363,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>51</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>52</v>
       </c>
@@ -1382,7 +1385,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>53</v>
       </c>
@@ -1393,7 +1396,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
@@ -1404,7 +1407,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>55</v>
       </c>
@@ -1415,7 +1418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>59</v>
       </c>
@@ -1426,7 +1429,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>60</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>61</v>
       </c>
@@ -1448,7 +1451,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>62</v>
       </c>
@@ -1459,7 +1462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>63</v>
       </c>
@@ -1470,7 +1473,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>64</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>65</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>66</v>
       </c>
@@ -1503,7 +1506,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>67</v>
       </c>
@@ -1514,7 +1517,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>71</v>
       </c>
@@ -1525,7 +1528,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>72</v>
       </c>
@@ -1536,7 +1539,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>73</v>
       </c>
@@ -1547,7 +1550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>74</v>
       </c>
@@ -1558,7 +1561,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>75</v>
       </c>
@@ -1569,7 +1572,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>76</v>
       </c>
@@ -1580,7 +1583,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>77</v>
       </c>
@@ -1591,7 +1594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>78</v>
       </c>
@@ -1602,7 +1605,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>79</v>
       </c>
@@ -1613,7 +1616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>80</v>
       </c>
@@ -1624,7 +1627,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>81</v>
       </c>
@@ -1635,7 +1638,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>82</v>
       </c>
@@ -1646,7 +1649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>83</v>
       </c>
@@ -1657,7 +1660,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>84</v>
       </c>
@@ -1668,7 +1671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>85</v>
       </c>
@@ -1679,7 +1682,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>86</v>
       </c>
@@ -1690,7 +1693,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>41</v>
       </c>
@@ -1701,7 +1704,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>87</v>
       </c>
@@ -1712,7 +1715,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>88</v>
       </c>
@@ -1723,7 +1726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>89</v>
       </c>
@@ -1734,7 +1737,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>90</v>
       </c>
@@ -1745,7 +1748,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>91</v>
       </c>
@@ -1756,7 +1759,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>92</v>
       </c>
@@ -1767,7 +1770,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>93</v>
       </c>
@@ -1778,7 +1781,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>94</v>
       </c>
@@ -1789,7 +1792,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>95</v>
       </c>
@@ -1800,7 +1803,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>96</v>
       </c>
@@ -1811,7 +1814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>97</v>
       </c>
@@ -1822,7 +1825,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>98</v>
       </c>
@@ -1833,7 +1836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" s="5" t="s">
         <v>101</v>
       </c>
@@ -1844,7 +1847,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="5" t="s">
         <v>104</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="5" t="s">
         <v>105</v>
       </c>
@@ -1866,7 +1869,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="5" t="s">
         <v>107</v>
       </c>
@@ -1877,7 +1880,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" s="5" t="s">
         <v>108</v>
       </c>
@@ -1888,7 +1891,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" s="5" t="s">
         <v>109</v>
       </c>
@@ -1899,7 +1902,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" s="5" t="s">
         <v>110</v>
       </c>
@@ -1910,7 +1913,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" s="5" t="s">
         <v>111</v>
       </c>
@@ -1921,7 +1924,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" s="5" t="s">
         <v>112</v>
       </c>
@@ -1932,7 +1935,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="5" t="s">
         <v>113</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
         <v>114</v>
       </c>
@@ -1954,7 +1957,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
         <v>115</v>
       </c>
@@ -1965,7 +1968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
         <v>116</v>
       </c>
@@ -1976,7 +1979,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
         <v>117</v>
       </c>
@@ -1987,7 +1990,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
         <v>118</v>
       </c>
@@ -1998,7 +2001,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
         <v>119</v>
       </c>
@@ -2009,7 +2012,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
         <v>120</v>
       </c>
@@ -2020,7 +2023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
         <v>121</v>
       </c>
@@ -2031,7 +2034,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
         <v>122</v>
       </c>
@@ -2042,7 +2045,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" s="5" t="s">
         <v>123</v>
       </c>
@@ -2053,7 +2056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" s="5" t="s">
         <v>124</v>
       </c>
@@ -2062,7 +2065,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" s="5" t="s">
         <v>125</v>
       </c>
@@ -2073,7 +2076,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
         <v>126</v>
       </c>
@@ -2084,7 +2087,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" s="5" t="s">
         <v>127</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" s="5" t="s">
         <v>128</v>
       </c>
@@ -2106,7 +2109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" s="5" t="s">
         <v>129</v>
       </c>
@@ -2117,7 +2120,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
         <v>130</v>
       </c>
@@ -2128,7 +2131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
         <v>131</v>
       </c>
@@ -2139,7 +2142,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" s="5" t="s">
         <v>132</v>
       </c>
@@ -2158,14 +2161,535 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6325C14E-3CC7-406C-AE5A-8C7D59A52FFD}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B51">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B56">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B58">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B63">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65">
+        <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2178,24 +2702,24 @@
       <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>102</v>
       </c>

</xml_diff>